<commit_message>
add updated training model script
</commit_message>
<xml_diff>
--- a/data/filenames-indexes.xlsx
+++ b/data/filenames-indexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikol/Desktop/engrCapst/ExoArm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E932E-FDFC-D34E-86CA-2C1D6EF2B314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48985FC6-043D-1B4A-AB66-D6E25BC8C4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
     <t>../data/CoolTerm Capture 2022-12-06 20-02-36.txt</t>
   </si>
   <si>
-    <t>../data/TEST.txt</t>
+    <t>../data/CoolTerm Capture 2023-02-02 10-56-19.txt</t>
   </si>
 </sst>
 </file>
@@ -77,7 +77,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -653,6 +652,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -746,10 +748,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E14"/>
+      <selection activeCell="E7" sqref="D6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -776,16 +781,16 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1530</v>
+        <v>356</v>
       </c>
       <c r="C2">
-        <v>872</v>
+        <v>1314</v>
       </c>
       <c r="D2">
-        <v>629</v>
+        <v>2669</v>
       </c>
       <c r="E2">
-        <v>975</v>
+        <v>2008</v>
       </c>
       <c r="F2">
         <v>90</v>
@@ -793,44 +798,44 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>1460</v>
+        <v>620</v>
       </c>
       <c r="C3">
-        <v>1645</v>
+        <v>1512</v>
       </c>
       <c r="D3">
-        <v>1325</v>
+        <v>2769</v>
       </c>
       <c r="E3">
-        <v>1765</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>2084</v>
+        <v>818</v>
       </c>
       <c r="C4">
-        <v>2452</v>
+        <v>1678</v>
       </c>
       <c r="D4">
-        <v>2166</v>
+        <v>2967</v>
       </c>
       <c r="E4">
-        <v>2568</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>100</v>
+        <v>1182</v>
       </c>
       <c r="C5">
-        <v>3098</v>
+        <v>1843</v>
       </c>
       <c r="D5">
-        <v>2860</v>
+        <v>3033</v>
       </c>
       <c r="E5">
-        <v>3210</v>
+        <v>2471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add arduino impl of match filtering
</commit_message>
<xml_diff>
--- a/data/filenames-indexes.xlsx
+++ b/data/filenames-indexes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikol/Desktop/engrCapst/ExoArm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3F4E84-5512-8B4D-9A73-60DFB4EB41F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B356D810-3A77-9C4F-9536-CB99645803F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet7" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
@@ -582,10 +582,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>356</v>
+      </c>
+      <c r="C2">
+        <v>1314</v>
+      </c>
+      <c r="D2">
+        <v>2729</v>
+      </c>
+      <c r="E2">
+        <v>2008</v>
+      </c>
+      <c r="F2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>620</v>
+      </c>
+      <c r="C3">
+        <v>1512</v>
+      </c>
+      <c r="D3">
+        <v>2769</v>
+      </c>
+      <c r="E3">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>818</v>
+      </c>
+      <c r="C4">
+        <v>1678</v>
+      </c>
+      <c r="D4">
+        <v>3027</v>
+      </c>
+      <c r="E4">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1182</v>
+      </c>
+      <c r="C5">
+        <v>1843</v>
+      </c>
+      <c r="D5">
+        <v>3033</v>
+      </c>
+      <c r="E5">
+        <v>2471</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -882,7 +982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1094,106 +1194,6 @@
       </c>
       <c r="C15">
         <v>7875</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>356</v>
-      </c>
-      <c r="C2">
-        <v>1314</v>
-      </c>
-      <c r="D2">
-        <v>2669</v>
-      </c>
-      <c r="E2">
-        <v>2008</v>
-      </c>
-      <c r="F2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>620</v>
-      </c>
-      <c r="C3">
-        <v>1512</v>
-      </c>
-      <c r="D3">
-        <v>2769</v>
-      </c>
-      <c r="E3">
-        <v>2273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>818</v>
-      </c>
-      <c r="C4">
-        <v>1678</v>
-      </c>
-      <c r="D4">
-        <v>2967</v>
-      </c>
-      <c r="E4">
-        <v>2372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>1182</v>
-      </c>
-      <c r="C5">
-        <v>1843</v>
-      </c>
-      <c r="D5">
-        <v>3033</v>
-      </c>
-      <c r="E5">
-        <v>2471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>